<commit_message>
* Changes for the parsing and execution of V2 Commands (INCOMPLETE) * Minor refactorings
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/test_spreadsheet_3_dataset.xlsx
+++ b/backend_tests/z_input_files/test_spreadsheet_3_dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
   <si>
     <t xml:space="preserve">Case study code</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t xml:space="preserve">Authors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maddalena Ripa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafael Nebot</t>
   </si>
   <si>
     <t xml:space="preserve">Date of elaboration</t>
@@ -572,17 +578,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,10 +653,16 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>2018</v>
@@ -658,7 +670,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2013</v>
@@ -666,45 +678,45 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -719,23 +731,23 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,7 +755,7 @@
         <v>2100</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,7 +763,7 @@
         <v>2200</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,7 +771,7 @@
         <v>2410</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -767,7 +779,7 @@
         <v>3214</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,7 +787,7 @@
         <v>3215</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +795,7 @@
         <v>3215</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,7 +803,7 @@
         <v>3220</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,7 +811,7 @@
         <v>3234</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -807,7 +819,7 @@
         <v>3235</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,7 +827,7 @@
         <v>3244</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,7 +835,7 @@
         <v>3246</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,7 +843,7 @@
         <v>3247</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,7 +851,7 @@
         <v>3250</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,15 +859,15 @@
         <v>3260</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,7 +875,7 @@
         <v>3280</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -871,7 +883,7 @@
         <v>3285</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,7 +891,7 @@
         <v>4000</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +899,7 @@
         <v>5532</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,7 +907,7 @@
         <v>5541</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +915,7 @@
         <v>5542</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -911,7 +923,7 @@
         <v>55431</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,7 +931,7 @@
         <v>55432</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,7 +939,7 @@
         <v>5544</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,7 +947,7 @@
         <v>5545</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -943,7 +955,7 @@
         <v>5550</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -951,7 +963,7 @@
         <v>6000</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,7 +971,7 @@
         <v>7100</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,13 +979,13 @@
         <v>7200</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -988,165 +1000,165 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1161,65 +1173,64 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="N1" s="0" t="s">
         <v>10</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>2012</v>
@@ -1228,198 +1239,198 @@
         <v>2012</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K6" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K7" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K8" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K10" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K11" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K12" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K15" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K16" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K17" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K18" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1434,20 +1445,20 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="8.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.37"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,57 +1466,57 @@
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1520,76 +1531,76 @@
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="4" width="7.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="4" width="7.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="8.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="4" width="10.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="4" width="7.56"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="4" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="4" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="4" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="4" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="0"/>
       <c r="C1" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="H1" s="0"/>
       <c r="I1" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J1" s="0"/>
       <c r="K1" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
       <c r="I2" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K2" s="4" t="n">
         <v>2012</v>
@@ -1598,62 +1609,62 @@
         <v>2012</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
* Created empty implementation of "version 2" of commands * Implementation of command "hierarchy_categories_command.py" * Modification of helpers in "spreadsheet_command_parsers_v2.__init__.py" * "basic_elements_parser.py": fix rule for "unquoted_string"; "code_string" (a code in a category hierarchy) modified to support "_" (underscore) * Refactoring of names of parser modules: parser_json.py, parser_spreadsheet.py, ... * "musiasem_concepts.py" incorporates a model for in-memory datasets similar to the SDMX model. Other minor changes * "serialization.py" fixes a problem preventing losing in-memory state when serializing it (slows execution because it clones) * "command_field_definitions.py" commented out lines just to allow the system work
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/test_spreadsheet_3_dataset.xlsx
+++ b/backend_tests/z_input_files/test_spreadsheet_3_dataset.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author/>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -392,7 +392,7 @@
     <t xml:space="preserve">#MuSIASEM_EC</t>
   </si>
   <si>
-    <t xml:space="preserve">#VALUE</t>
+    <t xml:space="preserve">#SUM_VALUE</t>
   </si>
   <si>
     <t xml:space="preserve">#Time_period</t>
@@ -580,15 +580,15 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -716,7 +716,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -731,15 +731,15 @@
   </sheetPr>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,7 +985,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1000,15 +1000,15 @@
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,7 +1158,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1173,21 +1173,22 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,7 +1431,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1445,20 +1446,20 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.23"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1517,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1531,19 +1532,19 @@
   </sheetPr>
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q3" activeCellId="0" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="4" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="4" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="4" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="4" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="4" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="4" width="7.4234693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="4" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="9" style="4" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="4" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="4" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="4" width="7.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1664,7 +1665,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>